<commit_message>
ExcelImportSeeder-DatabaseSeeder update table relations
</commit_message>
<xml_diff>
--- a/public/Excel/course_field.xlsx
+++ b/public/Excel/course_field.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B5F84D7-8C50-47FD-A17E-9C05EF9A50F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,33 +13,42 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_2" localSheetId="0" hidden="1">Sheet1!$A$1:$B$26</definedName>
+    <definedName name="ExternalData_2" localSheetId="0" hidden="1">Sheet1!$A$1:$B$8</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" keepAlive="1" name="Query - Table 3 (2)" description="Connection to the 'Table 3 (2)' query in the workbook." type="5" refreshedVersion="8" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" keepAlive="1" name="Query - Table 3 (2)" description="Connection to the 'Table 3 (2)' query in the workbook." type="5" refreshedVersion="8" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;Table 3 (2)&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [Table 3 (2)]"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
   <si>
-    <t>course_id</t>
+    <t>course_code</t>
   </si>
   <si>
-    <t>field_id</t>
+    <t>field_name</t>
+  </si>
+  <si>
+    <t>mobile</t>
+  </si>
+  <si>
+    <t>design</t>
+  </si>
+  <si>
+    <t>security</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -87,12 +97,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_2" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_2" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="7">
     <queryTableFields count="2">
       <queryTableField id="1" name="course number" tableColumnId="1"/>
@@ -107,11 +120,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table_3__2" displayName="Table_3__2" ref="A1:B26" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:B26"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_3__2" displayName="Table_3__2" ref="A1:B8" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:B8" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" uniqueName="1" name="course_id" queryTableFieldId="1" dataDxfId="1"/>
-    <tableColumn id="2" uniqueName="2" name="field_id" queryTableFieldId="2" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="course_code" queryTableFieldId="1" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="field_name" queryTableFieldId="2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -160,7 +173,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -193,9 +206,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -228,6 +258,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -403,17 +450,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -426,201 +474,57 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>3</v>
+        <v>4170210</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
+        <v>4170211</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
+        <v>4170212</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
+        <v>4170213</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6">
-        <v>3</v>
+        <v>4170214</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
+        <v>4170309</v>
+      </c>
+      <c r="B7" t="s">
         <v>3</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>3</v>
-      </c>
-      <c r="B8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>4</v>
-      </c>
-      <c r="B9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>4</v>
-      </c>
-      <c r="B10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>4</v>
-      </c>
-      <c r="B11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>4</v>
-      </c>
-      <c r="B12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>5</v>
-      </c>
-      <c r="B13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>5</v>
-      </c>
-      <c r="B14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>5</v>
-      </c>
-      <c r="B15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>5</v>
-      </c>
-      <c r="B16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>5</v>
-      </c>
-      <c r="B17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>6</v>
-      </c>
-      <c r="B18">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>6</v>
-      </c>
-      <c r="B19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>7</v>
-      </c>
-      <c r="B20">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>7</v>
-      </c>
-      <c r="B21">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>7</v>
-      </c>
-      <c r="B22">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>8</v>
-      </c>
-      <c r="B23">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <v>8</v>
-      </c>
-      <c r="B24">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>8</v>
-      </c>
-      <c r="B25">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>9</v>
-      </c>
-      <c r="B26">
+        <v>4170208</v>
+      </c>
+      <c r="B8" t="s">
         <v>3</v>
       </c>
     </row>
@@ -633,7 +537,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -645,7 +549,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>